<commit_message>
fixing typo in behavior log
</commit_message>
<xml_diff>
--- a/Mario_Behavior_Log.xlsx
+++ b/Mario_Behavior_Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8340" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8340" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Log" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7861" uniqueCount="3490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7861" uniqueCount="3491">
   <si>
     <t xml:space="preserve">Session </t>
   </si>
@@ -10495,6 +10495,9 @@
   </si>
   <si>
     <t>Checking array after ~2 months without plugging animal in. See units on: 2, 6, 8, 23, 28, 45, 65, 66, 71, 74, 76, 78, 81, 82, 84, 89, 104, 110, 113, 116, 117, 118, 120, 121, 122, 123, 124. Noisy channels: 1, 10, 12, 14, 16, 47, 49, 52, 54, 59, 61, 63, 67, 80, 93, 95, 97, 98, 99, 103, 111,112, 125, 127, 135, 146, 157, 159. Checked eye-tracker system and found that it's stilll working well.</t>
+  </si>
+  <si>
+    <t>Mario20160716-Block1</t>
   </si>
 </sst>
 </file>
@@ -48582,7 +48585,7 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -52731,7 +52734,9 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -53209,7 +53214,7 @@
         <v>623</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>625</v>
+        <v>3490</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>380</v>

</xml_diff>

<commit_message>
fixing typo in log
</commit_message>
<xml_diff>
--- a/Mario_Behavior_Log.xlsx
+++ b/Mario_Behavior_Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8340" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8340" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Log" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7854" uniqueCount="3490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7854" uniqueCount="3491">
   <si>
     <t xml:space="preserve">Session </t>
   </si>
@@ -10495,6 +10495,9 @@
   </si>
   <si>
     <t>Mario20160716-Block1</t>
+  </si>
+  <si>
+    <t>mari20160317_08_te1760.hdf</t>
   </si>
 </sst>
 </file>
@@ -52731,7 +52734,7 @@
   </sheetPr>
   <dimension ref="A1:K999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -60273,7 +60276,9 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -60413,7 +60418,7 @@
         <v>1275</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1277</v>
+        <v>3490</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1278</v>

</xml_diff>

<commit_message>
changes for doing baseline firing rate comps across sessions
</commit_message>
<xml_diff>
--- a/Mario_Behavior_Log.xlsx
+++ b/Mario_Behavior_Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="8340" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Log" sheetId="1" r:id="rId1"/>
@@ -10474,63 +10474,75 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -10974,8 +10986,8 @@
   <dimension ref="A1:AI2034"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="4" topLeftCell="A1529" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1551" sqref="I1551"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -46707,8 +46719,8 @@
   </sheetPr>
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -47496,8 +47508,8 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:AC39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -47515,7 +47527,7 @@
         <v>3476</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>

</xml_diff>